<commit_message>
changed textfeilds to buttons for somepages
</commit_message>
<xml_diff>
--- a/resources/1st.xlsx
+++ b/resources/1st.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,7 +15,7 @@
     <sheet name="Involved Learners (IL)" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -54,7 +55,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -417,15 +418,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1"/>
+    <row r="2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -437,13 +439,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K3"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -498,68 +500,20 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Manoj</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Varad</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>9/12/2023</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>LDFDLFJLKS</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>KSKFJHOS87789</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>A+</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -572,13 +526,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -632,58 +586,17 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Manoj</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>180</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>63</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>something</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>7th Jan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>me</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>red</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>mango</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>dog</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>neem</t>
-        </is>
-      </c>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -696,85 +609,117 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>HW 4.10</t>
+          <t>HW 4.10 term 1</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>HW 4.11</t>
+          <t>HW 4.10 term 2</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>HW 4.7</t>
+          <t>HW 4.11 term 1</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>HW 5.8</t>
+          <t>HW 4.11 term 2</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>HW 5.13A</t>
+          <t>HW 4.7 term 1</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>HW 5.13a</t>
+          <t>HW 4.7 term 2</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>HW 5.16</t>
+          <t>HW 5.8 term 1</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>HW 5.17</t>
+          <t>HW 5.8 term 2</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>HW 5.18a</t>
+          <t>HW 5.13A term 1</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>HW 5.18b</t>
+          <t>HW 5.13A term 2</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>HW 5.13a term 1</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>HW 5.13a term 2</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>HW 5.16 term 1</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>HW 5.16 term 2</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>HW 5.17 term 1</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>HW 5.17 term 2</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>HW 5.18a term 1</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>HW 5.18a term 2</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>HW 5.18b term 1</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>HW 5.18b term 2</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Beginer</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-    </row>
+    <row r="2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -786,85 +731,127 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ECL 15.4</t>
+          <t>ECL 15.4 term 1</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>ECL 15.5a</t>
+          <t>ECL 15.4 term 2</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>ECL 15.5b</t>
+          <t>ECL 15.5a term 1</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>ECL 15.5c</t>
+          <t>ECL 15.5a term 2</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>ECL 15.7</t>
+          <t>ECL 15.5b term 1</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>ECL 15.8</t>
+          <t>ECL 15.5b term 2</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>ECL 15.9</t>
+          <t>ECL 15.5c term 1</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>ECL 2-5.10</t>
+          <t>ECL 15.5c term 2</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>ECL 2-5.12</t>
+          <t>ECL 15.7 term 1</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>ECL 2-5.1a</t>
+          <t>ECL 15.7 term 2</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>ECL 2-5.2</t>
+          <t>ECL 15.8 term 1</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>ECL 15.8 term 2</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>ECL 15.9 term 1</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>ECL 15.9 term 2</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>ECL 2-5.10 term 1</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>ECL 2-5.10 term 2</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>ECL 2-5.12 term 1</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>ECL 2-5.12 term 2</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>ECL 2-5.1a term 1</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>ECL 2-5.1a term 2</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>ECL 2-5.2 term 1</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>ECL 2-5.2 term 2</t>
         </is>
       </c>
     </row>
     <row r="2"/>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -876,97 +863,147 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>IL 4.1</t>
+          <t>IL 4.1 term 1</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>IL 4.2a</t>
+          <t>IL 4.1 term 2</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>IL 4.8c</t>
+          <t>IL 4.2a term 1</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>IL 4.6</t>
+          <t>IL 4.2a term 2</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>IL 4.11</t>
+          <t>IL 4.8c term 1</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>IL 4.13</t>
+          <t>IL 4.8c term 2</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>IL 4.16</t>
+          <t>IL 4.6 term 1</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>IL 4.9</t>
+          <t>IL 4.6 term 2</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>IL 4.20</t>
+          <t>IL 4.11 term 1</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>IL 4.25</t>
+          <t>IL 4.11 term 2</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>IL 4.27</t>
+          <t>IL 4.13 term 1</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>IL 4.29</t>
+          <t>IL 4.13 term 2</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>IL 4.30</t>
+          <t>IL 4.16 term 1</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>IL 4.16 term 2</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>IL 4.9 term 1</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>IL 4.9 term 2</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>IL 4.20 term 1</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>IL 4.20 term 2</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>IL 4.25 term 1</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>IL 4.25 term 2</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>IL 4.27 term 1</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>IL 4.27 term 2</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>IL 4.29 term 1</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>IL 4.29 term 2</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>IL 4.30 term 1</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>IL 4.30 term 2</t>
         </is>
       </c>
     </row>
     <row r="2"/>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added section_no to AddScreen
</commit_message>
<xml_diff>
--- a/resources/1st.xlsx
+++ b/resources/1st.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="A2:B2"/>
@@ -428,7 +428,6 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1"/>
-    <row r="3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -440,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
@@ -565,16 +564,9 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>07/01/2003</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+          <t>07/01/2004</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -672,6 +664,26 @@
           <t>45</t>
         </is>
       </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Thapa</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -684,7 +696,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -802,15 +814,6 @@
           <t>Manoj</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -823,6 +826,18 @@
           <t>resources/images//Me.png</t>
         </is>
       </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -835,7 +850,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:D4"/>
@@ -972,6 +987,18 @@
       <c r="B12" t="inlineStr">
         <is>
           <t>resources/images/45/Me.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>resources/images/57/Family.jpg</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>resources/images/57/Me.png</t>
         </is>
       </c>
     </row>
@@ -986,7 +1013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
@@ -1198,27 +1225,28 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
+    <row r="3"/>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1231,7 +1259,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1463,29 +1491,30 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
+    <row r="3"/>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1498,7 +1527,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
@@ -1770,34 +1799,7 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-    </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
@@ -1844,6 +1846,34 @@
           <t>None</t>
         </is>
       </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1856,7 +1886,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
@@ -2381,6 +2411,53 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>